<commit_message>
[Update] Create Job Excel and JWT token Handler
</commit_message>
<xml_diff>
--- a/JobCategory.xlsx
+++ b/JobCategory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lee\Desktop\yensoserver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91161D42-5A2D-4407-83B3-FE9D794B09EF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2C71C8-79DB-4B8B-88D7-C8A8B2B6FA94}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10747" xr2:uid="{C3208E4A-6860-4D74-991E-A292A8CD4705}"/>
   </bookViews>
@@ -443,9 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A57C68-EB4F-4C7A-AB2F-CDABAFEF9F3F}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A9:A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.350000000000001"/>
   <cols>

</xml_diff>